<commit_message>
construct multivariate table for analysis, continue working on some scripts
</commit_message>
<xml_diff>
--- a/Data/9month-size-backup.xlsx
+++ b/Data/9month-size-backup.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28331"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/studentuser/Desktop/Laura/O.lurida_Stress/Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8DB3A5-FCB4-AF46-A67C-A8573C3DC1E2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="25360" windowHeight="15220" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="25360" windowHeight="15220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9-month Size" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Laura Spencer</author>
   </authors>
   <commentList>
-    <comment ref="S117" authorId="0">
+    <comment ref="S117" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -54,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1466" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="83">
   <si>
     <t>GROUP</t>
   </si>
@@ -301,11 +307,14 @@
   <si>
     <t>SN6-LOW-Exp</t>
   </si>
+  <si>
+    <t xml:space="preserve">These were added to the dataset as size = 2mm </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -419,6 +428,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -743,22 +760,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ323"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AJ331"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A252" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="G274" sqref="G274"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" customWidth="1"/>
     <col min="3" max="6" width="10.83203125" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="11" max="11" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -788,7 +806,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="2:11" s="2" customFormat="1">
+    <row r="2" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
@@ -820,7 +838,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:11" s="2" customFormat="1">
+    <row r="3" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
@@ -848,8 +866,11 @@
         <v>272.75</v>
       </c>
       <c r="I3" s="6"/>
-    </row>
-    <row r="4" spans="2:11">
+      <c r="K3" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>12</v>
       </c>
@@ -878,7 +899,7 @@
       </c>
       <c r="I4" s="11"/>
     </row>
-    <row r="5" spans="2:11">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>13</v>
       </c>
@@ -907,7 +928,7 @@
       </c>
       <c r="I5" s="11"/>
     </row>
-    <row r="6" spans="2:11" s="2" customFormat="1">
+    <row r="6" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
@@ -936,7 +957,7 @@
       </c>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="2:11" s="2" customFormat="1">
+    <row r="7" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
@@ -965,7 +986,7 @@
       </c>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="2:11">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>16</v>
       </c>
@@ -994,7 +1015,7 @@
       </c>
       <c r="I8" s="11"/>
     </row>
-    <row r="9" spans="2:11">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>17</v>
       </c>
@@ -1023,7 +1044,7 @@
       </c>
       <c r="I9" s="11"/>
     </row>
-    <row r="10" spans="2:11">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>18</v>
       </c>
@@ -1052,7 +1073,7 @@
       </c>
       <c r="I10" s="11"/>
     </row>
-    <row r="11" spans="2:11">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>19</v>
       </c>
@@ -1081,7 +1102,7 @@
       </c>
       <c r="I11" s="11"/>
     </row>
-    <row r="12" spans="2:11" s="2" customFormat="1">
+    <row r="12" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>20</v>
       </c>
@@ -1110,7 +1131,7 @@
       </c>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="2:11">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>21</v>
       </c>
@@ -1139,7 +1160,7 @@
       </c>
       <c r="I13" s="11"/>
     </row>
-    <row r="14" spans="2:11">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>22</v>
       </c>
@@ -1168,7 +1189,7 @@
       </c>
       <c r="I14" s="11"/>
     </row>
-    <row r="15" spans="2:11">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>23</v>
       </c>
@@ -1197,7 +1218,7 @@
       </c>
       <c r="I15" s="11"/>
     </row>
-    <row r="16" spans="2:11">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>24</v>
       </c>
@@ -1226,7 +1247,7 @@
       </c>
       <c r="I16" s="11"/>
     </row>
-    <row r="17" spans="1:36">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>25</v>
       </c>
@@ -1255,7 +1276,7 @@
       </c>
       <c r="I17" s="11"/>
     </row>
-    <row r="19" spans="1:36">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>26</v>
       </c>
@@ -1356,7 +1377,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:36">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>58</v>
       </c>
@@ -1436,7 +1457,7 @@
         <v>4.07</v>
       </c>
     </row>
-    <row r="21" spans="1:36">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -1516,7 +1537,7 @@
         <v>3.27</v>
       </c>
     </row>
-    <row r="22" spans="1:36">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>58</v>
       </c>
@@ -1596,7 +1617,7 @@
         <v>7.76</v>
       </c>
     </row>
-    <row r="23" spans="1:36">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>58</v>
       </c>
@@ -1676,7 +1697,7 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="24" spans="1:36">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>58</v>
       </c>
@@ -1756,7 +1777,7 @@
         <v>5.53</v>
       </c>
     </row>
-    <row r="25" spans="1:36">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>58</v>
       </c>
@@ -1836,7 +1857,7 @@
         <v>11.33</v>
       </c>
     </row>
-    <row r="26" spans="1:36">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>58</v>
       </c>
@@ -1916,7 +1937,7 @@
         <v>5.62</v>
       </c>
     </row>
-    <row r="27" spans="1:36">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>58</v>
       </c>
@@ -1996,7 +2017,7 @@
         <v>4.76</v>
       </c>
     </row>
-    <row r="28" spans="1:36">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>58</v>
       </c>
@@ -2076,7 +2097,7 @@
         <v>7.08</v>
       </c>
     </row>
-    <row r="29" spans="1:36">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>58</v>
       </c>
@@ -2156,7 +2177,7 @@
         <v>5.37</v>
       </c>
     </row>
-    <row r="30" spans="1:36">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>2</v>
       </c>
@@ -2252,7 +2273,7 @@
         <v>6.9299999999999988</v>
       </c>
     </row>
-    <row r="31" spans="1:36">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>49</v>
       </c>
@@ -2332,7 +2353,7 @@
       <c r="AI31" s="1"/>
       <c r="AJ31" s="1"/>
     </row>
-    <row r="32" spans="1:36">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>50</v>
       </c>
@@ -2397,7 +2418,7 @@
         <v>6.77</v>
       </c>
     </row>
-    <row r="33" spans="1:36">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>51</v>
       </c>
@@ -2462,7 +2483,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="34" spans="1:36">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>52</v>
       </c>
@@ -2527,7 +2548,7 @@
         <v>6.59</v>
       </c>
     </row>
-    <row r="35" spans="1:36">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>53</v>
       </c>
@@ -2592,7 +2613,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="36" spans="1:36">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>54</v>
       </c>
@@ -2657,7 +2678,7 @@
         <v>6.87</v>
       </c>
     </row>
-    <row r="37" spans="1:36">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>55</v>
       </c>
@@ -2722,7 +2743,7 @@
         <v>5.26</v>
       </c>
     </row>
-    <row r="38" spans="1:36">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>56</v>
       </c>
@@ -2787,7 +2808,7 @@
         <v>6.05</v>
       </c>
     </row>
-    <row r="39" spans="1:36">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>57</v>
       </c>
@@ -2852,7 +2873,7 @@
         <v>6.48</v>
       </c>
     </row>
-    <row r="40" spans="1:36">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>58</v>
       </c>
@@ -2917,7 +2938,7 @@
         <v>5.48</v>
       </c>
     </row>
-    <row r="41" spans="1:36">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>59</v>
       </c>
@@ -2982,7 +3003,7 @@
         <v>6.26</v>
       </c>
     </row>
-    <row r="42" spans="1:36">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>60</v>
       </c>
@@ -3047,7 +3068,7 @@
         <v>6.51</v>
       </c>
     </row>
-    <row r="43" spans="1:36">
+    <row r="43" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>61</v>
       </c>
@@ -3127,7 +3148,7 @@
       <c r="AI43" s="1"/>
       <c r="AJ43" s="1"/>
     </row>
-    <row r="44" spans="1:36">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>62</v>
       </c>
@@ -3192,7 +3213,7 @@
         <v>8.77</v>
       </c>
     </row>
-    <row r="45" spans="1:36">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>63</v>
       </c>
@@ -3257,7 +3278,7 @@
         <v>8.7799999999999994</v>
       </c>
     </row>
-    <row r="46" spans="1:36">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>64</v>
       </c>
@@ -3322,7 +3343,7 @@
         <v>7.84</v>
       </c>
     </row>
-    <row r="47" spans="1:36">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>65</v>
       </c>
@@ -3387,7 +3408,7 @@
         <v>10.43</v>
       </c>
     </row>
-    <row r="48" spans="1:36">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>66</v>
       </c>
@@ -3455,7 +3476,7 @@
         <v>7.24</v>
       </c>
     </row>
-    <row r="49" spans="1:36">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>67</v>
       </c>
@@ -3520,7 +3541,7 @@
         <v>7.07</v>
       </c>
     </row>
-    <row r="50" spans="1:36">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>68</v>
       </c>
@@ -3585,7 +3606,7 @@
         <v>9.6199999999999992</v>
       </c>
     </row>
-    <row r="51" spans="1:36">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>69</v>
       </c>
@@ -3650,7 +3671,7 @@
         <v>7.82</v>
       </c>
     </row>
-    <row r="52" spans="1:36">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>70</v>
       </c>
@@ -3715,7 +3736,7 @@
         <v>7.97</v>
       </c>
     </row>
-    <row r="53" spans="1:36">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>71</v>
       </c>
@@ -3780,7 +3801,7 @@
         <v>9.6199999999999992</v>
       </c>
     </row>
-    <row r="54" spans="1:36">
+    <row r="54" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>72</v>
       </c>
@@ -3845,7 +3866,7 @@
         <v>8.2200000000000006</v>
       </c>
     </row>
-    <row r="55" spans="1:36">
+    <row r="55" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>58</v>
       </c>
@@ -3925,7 +3946,7 @@
         <v>5.77</v>
       </c>
     </row>
-    <row r="56" spans="1:36">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>58</v>
       </c>
@@ -4005,7 +4026,7 @@
         <v>3.83</v>
       </c>
     </row>
-    <row r="57" spans="1:36">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>58</v>
       </c>
@@ -4085,7 +4106,7 @@
         <v>4.5599999999999996</v>
       </c>
     </row>
-    <row r="58" spans="1:36">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -4165,7 +4186,7 @@
         <v>5.92</v>
       </c>
     </row>
-    <row r="59" spans="1:36">
+    <row r="59" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -4245,7 +4266,7 @@
         <v>3.86</v>
       </c>
     </row>
-    <row r="60" spans="1:36">
+    <row r="60" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -4289,7 +4310,7 @@
         <v>3.97</v>
       </c>
     </row>
-    <row r="61" spans="1:36">
+    <row r="61" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>2</v>
       </c>
@@ -4385,7 +4406,7 @@
         <v>6.1792000000000016</v>
       </c>
     </row>
-    <row r="62" spans="1:36">
+    <row r="62" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>73</v>
       </c>
@@ -4465,7 +4486,7 @@
       <c r="AI62" s="1"/>
       <c r="AJ62" s="1"/>
     </row>
-    <row r="63" spans="1:36">
+    <row r="63" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>74</v>
       </c>
@@ -4530,7 +4551,7 @@
         <v>5.44</v>
       </c>
     </row>
-    <row r="64" spans="1:36">
+    <row r="64" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>75</v>
       </c>
@@ -4595,7 +4616,7 @@
         <v>4.87</v>
       </c>
     </row>
-    <row r="65" spans="1:36">
+    <row r="65" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>76</v>
       </c>
@@ -4660,7 +4681,7 @@
         <v>5.22</v>
       </c>
     </row>
-    <row r="66" spans="1:36">
+    <row r="66" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>77</v>
       </c>
@@ -4725,7 +4746,7 @@
         <v>5.63</v>
       </c>
     </row>
-    <row r="67" spans="1:36">
+    <row r="67" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>78</v>
       </c>
@@ -4790,7 +4811,7 @@
         <v>4.41</v>
       </c>
     </row>
-    <row r="68" spans="1:36">
+    <row r="68" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>79</v>
       </c>
@@ -4855,7 +4876,7 @@
         <v>5.23</v>
       </c>
     </row>
-    <row r="69" spans="1:36">
+    <row r="69" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>80</v>
       </c>
@@ -4920,7 +4941,7 @@
         <v>5.01</v>
       </c>
     </row>
-    <row r="70" spans="1:36">
+    <row r="70" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>81</v>
       </c>
@@ -4985,7 +5006,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="71" spans="1:36" s="1" customFormat="1">
+    <row r="71" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>82</v>
       </c>
@@ -5065,7 +5086,7 @@
       <c r="AI71"/>
       <c r="AJ71"/>
     </row>
-    <row r="72" spans="1:36">
+    <row r="72" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>83</v>
       </c>
@@ -5130,7 +5151,7 @@
         <v>5.37</v>
       </c>
     </row>
-    <row r="73" spans="1:36">
+    <row r="73" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>84</v>
       </c>
@@ -5195,7 +5216,7 @@
         <v>6.09</v>
       </c>
     </row>
-    <row r="74" spans="1:36">
+    <row r="74" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>85</v>
       </c>
@@ -5275,7 +5296,7 @@
       <c r="AI74" s="1"/>
       <c r="AJ74" s="1"/>
     </row>
-    <row r="75" spans="1:36">
+    <row r="75" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>86</v>
       </c>
@@ -5340,7 +5361,7 @@
         <v>10.210000000000001</v>
       </c>
     </row>
-    <row r="76" spans="1:36">
+    <row r="76" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>87</v>
       </c>
@@ -5405,7 +5426,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="77" spans="1:36">
+    <row r="77" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>88</v>
       </c>
@@ -5470,7 +5491,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="78" spans="1:36">
+    <row r="78" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>89</v>
       </c>
@@ -5535,7 +5556,7 @@
         <v>7.61</v>
       </c>
     </row>
-    <row r="79" spans="1:36">
+    <row r="79" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>90</v>
       </c>
@@ -5600,7 +5621,7 @@
         <v>7.07</v>
       </c>
     </row>
-    <row r="80" spans="1:36">
+    <row r="80" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>91</v>
       </c>
@@ -5665,7 +5686,7 @@
         <v>6.19</v>
       </c>
     </row>
-    <row r="81" spans="1:36">
+    <row r="81" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>92</v>
       </c>
@@ -5730,7 +5751,7 @@
         <v>7.35</v>
       </c>
     </row>
-    <row r="82" spans="1:36">
+    <row r="82" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>93</v>
       </c>
@@ -5795,7 +5816,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="83" spans="1:36" s="1" customFormat="1">
+    <row r="83" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>94</v>
       </c>
@@ -5875,7 +5896,7 @@
       <c r="AI83"/>
       <c r="AJ83"/>
     </row>
-    <row r="84" spans="1:36">
+    <row r="84" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>95</v>
       </c>
@@ -5940,7 +5961,7 @@
         <v>6.08</v>
       </c>
     </row>
-    <row r="85" spans="1:36">
+    <row r="85" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>96</v>
       </c>
@@ -6005,7 +6026,7 @@
         <v>6.29</v>
       </c>
     </row>
-    <row r="86" spans="1:36">
+    <row r="86" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>58</v>
       </c>
@@ -6085,7 +6106,7 @@
         <v>5.15</v>
       </c>
     </row>
-    <row r="87" spans="1:36">
+    <row r="87" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>58</v>
       </c>
@@ -6165,7 +6186,7 @@
         <v>4.07</v>
       </c>
     </row>
-    <row r="88" spans="1:36">
+    <row r="88" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>58</v>
       </c>
@@ -6245,7 +6266,7 @@
         <v>3.66</v>
       </c>
     </row>
-    <row r="89" spans="1:36">
+    <row r="89" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>58</v>
       </c>
@@ -6325,7 +6346,7 @@
         <v>3.18</v>
       </c>
     </row>
-    <row r="90" spans="1:36">
+    <row r="90" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>58</v>
       </c>
@@ -6405,7 +6426,7 @@
         <v>3.46</v>
       </c>
     </row>
-    <row r="91" spans="1:36">
+    <row r="91" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>2</v>
       </c>
@@ -6505,7 +6526,7 @@
       <c r="AI91" s="2"/>
       <c r="AJ91" s="2"/>
     </row>
-    <row r="92" spans="1:36">
+    <row r="92" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>159</v>
       </c>
@@ -6581,7 +6602,7 @@
       <c r="AI92" s="2"/>
       <c r="AJ92" s="2"/>
     </row>
-    <row r="93" spans="1:36">
+    <row r="93" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>160</v>
       </c>
@@ -6657,7 +6678,7 @@
       <c r="AI93" s="2"/>
       <c r="AJ93" s="2"/>
     </row>
-    <row r="94" spans="1:36">
+    <row r="94" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>161</v>
       </c>
@@ -6733,7 +6754,7 @@
       <c r="AI94" s="2"/>
       <c r="AJ94" s="2"/>
     </row>
-    <row r="95" spans="1:36">
+    <row r="95" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>162</v>
       </c>
@@ -6809,7 +6830,7 @@
       <c r="AI95" s="2"/>
       <c r="AJ95" s="2"/>
     </row>
-    <row r="96" spans="1:36" s="1" customFormat="1">
+    <row r="96" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>163</v>
       </c>
@@ -6885,7 +6906,7 @@
       <c r="AI96" s="2"/>
       <c r="AJ96" s="2"/>
     </row>
-    <row r="97" spans="1:36">
+    <row r="97" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>164</v>
       </c>
@@ -6961,7 +6982,7 @@
       <c r="AI97" s="2"/>
       <c r="AJ97" s="2"/>
     </row>
-    <row r="98" spans="1:36">
+    <row r="98" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>165</v>
       </c>
@@ -7037,7 +7058,7 @@
       <c r="AI98" s="2"/>
       <c r="AJ98" s="2"/>
     </row>
-    <row r="99" spans="1:36">
+    <row r="99" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>166</v>
       </c>
@@ -7113,7 +7134,7 @@
       <c r="AI99" s="2"/>
       <c r="AJ99" s="2"/>
     </row>
-    <row r="100" spans="1:36">
+    <row r="100" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>167</v>
       </c>
@@ -7189,7 +7210,7 @@
       <c r="AI100" s="2"/>
       <c r="AJ100" s="2"/>
     </row>
-    <row r="101" spans="1:36">
+    <row r="101" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>168</v>
       </c>
@@ -7265,7 +7286,7 @@
       <c r="AI101" s="2"/>
       <c r="AJ101" s="2"/>
     </row>
-    <row r="102" spans="1:36">
+    <row r="102" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>169</v>
       </c>
@@ -7341,7 +7362,7 @@
       <c r="AI102" s="2"/>
       <c r="AJ102" s="2"/>
     </row>
-    <row r="103" spans="1:36">
+    <row r="103" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>170</v>
       </c>
@@ -7417,7 +7438,7 @@
       <c r="AI103" s="2"/>
       <c r="AJ103" s="2"/>
     </row>
-    <row r="104" spans="1:36">
+    <row r="104" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>171</v>
       </c>
@@ -7493,7 +7514,7 @@
       <c r="AI104" s="2"/>
       <c r="AJ104" s="2"/>
     </row>
-    <row r="105" spans="1:36">
+    <row r="105" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>172</v>
       </c>
@@ -7569,7 +7590,7 @@
       <c r="AI105" s="2"/>
       <c r="AJ105" s="2"/>
     </row>
-    <row r="106" spans="1:36">
+    <row r="106" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>173</v>
       </c>
@@ -7645,7 +7666,7 @@
       <c r="AI106" s="2"/>
       <c r="AJ106" s="2"/>
     </row>
-    <row r="107" spans="1:36">
+    <row r="107" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>174</v>
       </c>
@@ -7721,7 +7742,7 @@
       <c r="AI107" s="2"/>
       <c r="AJ107" s="2"/>
     </row>
-    <row r="108" spans="1:36" s="1" customFormat="1">
+    <row r="108" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>175</v>
       </c>
@@ -7797,7 +7818,7 @@
       <c r="AI108" s="2"/>
       <c r="AJ108" s="2"/>
     </row>
-    <row r="109" spans="1:36">
+    <row r="109" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>176</v>
       </c>
@@ -7873,7 +7894,7 @@
       <c r="AI109" s="2"/>
       <c r="AJ109" s="2"/>
     </row>
-    <row r="110" spans="1:36">
+    <row r="110" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>177</v>
       </c>
@@ -7949,7 +7970,7 @@
       <c r="AI110" s="2"/>
       <c r="AJ110" s="2"/>
     </row>
-    <row r="111" spans="1:36">
+    <row r="111" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
         <v>178</v>
       </c>
@@ -8025,7 +8046,7 @@
       <c r="AI111" s="2"/>
       <c r="AJ111" s="2"/>
     </row>
-    <row r="112" spans="1:36">
+    <row r="112" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>179</v>
       </c>
@@ -8101,7 +8122,7 @@
       <c r="AI112" s="2"/>
       <c r="AJ112" s="2"/>
     </row>
-    <row r="113" spans="1:36">
+    <row r="113" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
         <v>180</v>
       </c>
@@ -8177,7 +8198,7 @@
       <c r="AI113" s="2"/>
       <c r="AJ113" s="2"/>
     </row>
-    <row r="114" spans="1:36">
+    <row r="114" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>181</v>
       </c>
@@ -8253,7 +8274,7 @@
       <c r="AI114" s="2"/>
       <c r="AJ114" s="2"/>
     </row>
-    <row r="115" spans="1:36">
+    <row r="115" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
         <v>182</v>
       </c>
@@ -8329,7 +8350,7 @@
       <c r="AI115" s="2"/>
       <c r="AJ115" s="2"/>
     </row>
-    <row r="116" spans="1:36">
+    <row r="116" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>2</v>
       </c>
@@ -8429,7 +8450,7 @@
       <c r="AI116" s="2"/>
       <c r="AJ116" s="2"/>
     </row>
-    <row r="117" spans="1:36">
+    <row r="117" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
         <v>183</v>
       </c>
@@ -8505,7 +8526,7 @@
       <c r="AI117" s="2"/>
       <c r="AJ117" s="2"/>
     </row>
-    <row r="118" spans="1:36">
+    <row r="118" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
         <v>184</v>
       </c>
@@ -8581,7 +8602,7 @@
       <c r="AI118" s="2"/>
       <c r="AJ118" s="2"/>
     </row>
-    <row r="119" spans="1:36">
+    <row r="119" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
         <v>185</v>
       </c>
@@ -8657,7 +8678,7 @@
       <c r="AI119" s="2"/>
       <c r="AJ119" s="2"/>
     </row>
-    <row r="120" spans="1:36">
+    <row r="120" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>186</v>
       </c>
@@ -8733,7 +8754,7 @@
       <c r="AI120" s="2"/>
       <c r="AJ120" s="2"/>
     </row>
-    <row r="121" spans="1:36">
+    <row r="121" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
         <v>187</v>
       </c>
@@ -8809,7 +8830,7 @@
       <c r="AI121" s="2"/>
       <c r="AJ121" s="2"/>
     </row>
-    <row r="122" spans="1:36">
+    <row r="122" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
         <v>188</v>
       </c>
@@ -8885,7 +8906,7 @@
       <c r="AI122" s="2"/>
       <c r="AJ122" s="2"/>
     </row>
-    <row r="123" spans="1:36">
+    <row r="123" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
         <v>189</v>
       </c>
@@ -8961,7 +8982,7 @@
       <c r="AI123" s="2"/>
       <c r="AJ123" s="2"/>
     </row>
-    <row r="124" spans="1:36">
+    <row r="124" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
         <v>190</v>
       </c>
@@ -9037,7 +9058,7 @@
       <c r="AI124" s="2"/>
       <c r="AJ124" s="2"/>
     </row>
-    <row r="125" spans="1:36">
+    <row r="125" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
         <v>191</v>
       </c>
@@ -9113,7 +9134,7 @@
       <c r="AI125" s="2"/>
       <c r="AJ125" s="2"/>
     </row>
-    <row r="126" spans="1:36">
+    <row r="126" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
         <v>192</v>
       </c>
@@ -9189,7 +9210,7 @@
       <c r="AI126" s="2"/>
       <c r="AJ126" s="2"/>
     </row>
-    <row r="127" spans="1:36">
+    <row r="127" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A127" s="2">
         <v>193</v>
       </c>
@@ -9265,7 +9286,7 @@
       <c r="AI127" s="2"/>
       <c r="AJ127" s="2"/>
     </row>
-    <row r="128" spans="1:36">
+    <row r="128" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
         <v>194</v>
       </c>
@@ -9341,7 +9362,7 @@
       <c r="AI128" s="2"/>
       <c r="AJ128" s="2"/>
     </row>
-    <row r="129" spans="1:36">
+    <row r="129" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
         <v>195</v>
       </c>
@@ -9417,7 +9438,7 @@
       <c r="AI129" s="2"/>
       <c r="AJ129" s="2"/>
     </row>
-    <row r="130" spans="1:36">
+    <row r="130" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
         <v>196</v>
       </c>
@@ -9493,7 +9514,7 @@
       <c r="AI130" s="2"/>
       <c r="AJ130" s="2"/>
     </row>
-    <row r="131" spans="1:36">
+    <row r="131" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A131" s="2">
         <v>197</v>
       </c>
@@ -9569,7 +9590,7 @@
       <c r="AI131" s="2"/>
       <c r="AJ131" s="2"/>
     </row>
-    <row r="132" spans="1:36">
+    <row r="132" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A132" s="2">
         <v>198</v>
       </c>
@@ -9645,7 +9666,7 @@
       <c r="AI132" s="2"/>
       <c r="AJ132" s="2"/>
     </row>
-    <row r="133" spans="1:36">
+    <row r="133" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A133" s="2">
         <v>199</v>
       </c>
@@ -9721,7 +9742,7 @@
       <c r="AI133" s="2"/>
       <c r="AJ133" s="2"/>
     </row>
-    <row r="134" spans="1:36">
+    <row r="134" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A134" s="2">
         <v>200</v>
       </c>
@@ -9797,7 +9818,7 @@
       <c r="AI134" s="2"/>
       <c r="AJ134" s="2"/>
     </row>
-    <row r="135" spans="1:36">
+    <row r="135" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A135" s="2">
         <v>201</v>
       </c>
@@ -9873,7 +9894,7 @@
       <c r="AI135" s="2"/>
       <c r="AJ135" s="2"/>
     </row>
-    <row r="136" spans="1:36">
+    <row r="136" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A136" s="2">
         <v>202</v>
       </c>
@@ -9949,7 +9970,7 @@
       <c r="AI136" s="2"/>
       <c r="AJ136" s="2"/>
     </row>
-    <row r="137" spans="1:36">
+    <row r="137" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A137" s="2">
         <v>203</v>
       </c>
@@ -10025,7 +10046,7 @@
       <c r="AI137" s="2"/>
       <c r="AJ137" s="2"/>
     </row>
-    <row r="138" spans="1:36">
+    <row r="138" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A138" s="2">
         <v>204</v>
       </c>
@@ -10101,7 +10122,7 @@
       <c r="AI138" s="2"/>
       <c r="AJ138" s="2"/>
     </row>
-    <row r="139" spans="1:36">
+    <row r="139" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A139" s="2">
         <v>205</v>
       </c>
@@ -10177,7 +10198,7 @@
       <c r="AI139" s="2"/>
       <c r="AJ139" s="2"/>
     </row>
-    <row r="140" spans="1:36">
+    <row r="140" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A140" s="2">
         <v>206</v>
       </c>
@@ -10253,7 +10274,7 @@
       <c r="AI140" s="2"/>
       <c r="AJ140" s="2"/>
     </row>
-    <row r="141" spans="1:36">
+    <row r="141" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>58</v>
       </c>
@@ -10333,7 +10354,7 @@
         <v>4.9800000000000004</v>
       </c>
     </row>
-    <row r="142" spans="1:36">
+    <row r="142" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>58</v>
       </c>
@@ -10413,7 +10434,7 @@
         <v>8.81</v>
       </c>
     </row>
-    <row r="143" spans="1:36">
+    <row r="143" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>58</v>
       </c>
@@ -10493,7 +10514,7 @@
         <v>10.7</v>
       </c>
     </row>
-    <row r="144" spans="1:36">
+    <row r="144" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>58</v>
       </c>
@@ -10573,7 +10594,7 @@
         <v>9.5399999999999991</v>
       </c>
     </row>
-    <row r="145" spans="1:32">
+    <row r="145" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>58</v>
       </c>
@@ -10653,7 +10674,7 @@
         <v>5.95</v>
       </c>
     </row>
-    <row r="146" spans="1:32">
+    <row r="146" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>58</v>
       </c>
@@ -10733,7 +10754,7 @@
         <v>13.04</v>
       </c>
     </row>
-    <row r="147" spans="1:32">
+    <row r="147" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>58</v>
       </c>
@@ -10813,7 +10834,7 @@
         <v>14.05</v>
       </c>
     </row>
-    <row r="148" spans="1:32">
+    <row r="148" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>58</v>
       </c>
@@ -10893,7 +10914,7 @@
         <v>5.61</v>
       </c>
     </row>
-    <row r="149" spans="1:32">
+    <row r="149" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>58</v>
       </c>
@@ -10973,7 +10994,7 @@
         <v>7.32</v>
       </c>
     </row>
-    <row r="150" spans="1:32">
+    <row r="150" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>58</v>
       </c>
@@ -11053,7 +11074,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="151" spans="1:32">
+    <row r="151" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>58</v>
       </c>
@@ -11133,7 +11154,7 @@
         <v>20.82</v>
       </c>
     </row>
-    <row r="152" spans="1:32">
+    <row r="152" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>58</v>
       </c>
@@ -11213,7 +11234,7 @@
         <v>10.78</v>
       </c>
     </row>
-    <row r="153" spans="1:32">
+    <row r="153" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>58</v>
       </c>
@@ -11293,7 +11314,7 @@
         <v>7.05</v>
       </c>
     </row>
-    <row r="154" spans="1:32">
+    <row r="154" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>58</v>
       </c>
@@ -11355,7 +11376,7 @@
         <v>5.95</v>
       </c>
     </row>
-    <row r="155" spans="1:32">
+    <row r="155" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>2</v>
       </c>
@@ -11450,7 +11471,7 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="156" spans="1:32">
+    <row r="156" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>1</v>
       </c>
@@ -11515,7 +11536,7 @@
         <v>13.51</v>
       </c>
     </row>
-    <row r="157" spans="1:32">
+    <row r="157" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>2</v>
       </c>
@@ -11580,7 +11601,7 @@
         <v>11.51</v>
       </c>
     </row>
-    <row r="158" spans="1:32">
+    <row r="158" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>3</v>
       </c>
@@ -11645,7 +11666,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="159" spans="1:32">
+    <row r="159" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>4</v>
       </c>
@@ -11710,7 +11731,7 @@
         <v>15.53</v>
       </c>
     </row>
-    <row r="160" spans="1:32">
+    <row r="160" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>5</v>
       </c>
@@ -11775,7 +11796,7 @@
         <v>12.28</v>
       </c>
     </row>
-    <row r="161" spans="1:21">
+    <row r="161" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>6</v>
       </c>
@@ -11840,7 +11861,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="162" spans="1:21">
+    <row r="162" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>7</v>
       </c>
@@ -11905,7 +11926,7 @@
         <v>6.68</v>
       </c>
     </row>
-    <row r="163" spans="1:21">
+    <row r="163" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>8</v>
       </c>
@@ -11970,7 +11991,7 @@
         <v>7.99</v>
       </c>
     </row>
-    <row r="164" spans="1:21">
+    <row r="164" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>9</v>
       </c>
@@ -12035,7 +12056,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="165" spans="1:21">
+    <row r="165" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>10</v>
       </c>
@@ -12100,7 +12121,7 @@
         <v>7.88</v>
       </c>
     </row>
-    <row r="166" spans="1:21">
+    <row r="166" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>11</v>
       </c>
@@ -12165,7 +12186,7 @@
         <v>5.78</v>
       </c>
     </row>
-    <row r="167" spans="1:21">
+    <row r="167" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>12</v>
       </c>
@@ -12228,7 +12249,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="168" spans="1:21">
+    <row r="168" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>37</v>
       </c>
@@ -12293,7 +12314,7 @@
         <v>7.53</v>
       </c>
     </row>
-    <row r="169" spans="1:21">
+    <row r="169" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>38</v>
       </c>
@@ -12358,7 +12379,7 @@
         <v>8.11</v>
       </c>
     </row>
-    <row r="170" spans="1:21">
+    <row r="170" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>39</v>
       </c>
@@ -12423,7 +12444,7 @@
         <v>7.92</v>
       </c>
     </row>
-    <row r="171" spans="1:21">
+    <row r="171" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>40</v>
       </c>
@@ -12488,7 +12509,7 @@
         <v>7.88</v>
       </c>
     </row>
-    <row r="172" spans="1:21">
+    <row r="172" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>41</v>
       </c>
@@ -12553,7 +12574,7 @@
         <v>6.56</v>
       </c>
     </row>
-    <row r="173" spans="1:21">
+    <row r="173" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>42</v>
       </c>
@@ -12618,7 +12639,7 @@
         <v>6.56</v>
       </c>
     </row>
-    <row r="174" spans="1:21">
+    <row r="174" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>43</v>
       </c>
@@ -12683,7 +12704,7 @@
         <v>10.58</v>
       </c>
     </row>
-    <row r="175" spans="1:21">
+    <row r="175" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>44</v>
       </c>
@@ -12748,7 +12769,7 @@
         <v>12.46</v>
       </c>
     </row>
-    <row r="176" spans="1:21">
+    <row r="176" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>45</v>
       </c>
@@ -12813,7 +12834,7 @@
         <v>13.19</v>
       </c>
     </row>
-    <row r="177" spans="1:36">
+    <row r="177" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>46</v>
       </c>
@@ -12878,7 +12899,7 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="178" spans="1:36">
+    <row r="178" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>47</v>
       </c>
@@ -12943,7 +12964,7 @@
         <v>12.11</v>
       </c>
     </row>
-    <row r="179" spans="1:36">
+    <row r="179" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>48</v>
       </c>
@@ -13008,7 +13029,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="180" spans="1:36">
+    <row r="180" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>2</v>
       </c>
@@ -13106,7 +13127,7 @@
         <v>4.5199999999999996</v>
       </c>
     </row>
-    <row r="181" spans="1:36">
+    <row r="181" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>13</v>
       </c>
@@ -13171,7 +13192,7 @@
         <v>4.34</v>
       </c>
     </row>
-    <row r="182" spans="1:36">
+    <row r="182" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>14</v>
       </c>
@@ -13236,7 +13257,7 @@
         <v>5.27</v>
       </c>
     </row>
-    <row r="183" spans="1:36" s="2" customFormat="1">
+    <row r="183" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>15</v>
       </c>
@@ -13316,7 +13337,7 @@
       <c r="AI183"/>
       <c r="AJ183"/>
     </row>
-    <row r="184" spans="1:36" s="2" customFormat="1">
+    <row r="184" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>16</v>
       </c>
@@ -13396,7 +13417,7 @@
       <c r="AI184"/>
       <c r="AJ184"/>
     </row>
-    <row r="185" spans="1:36" s="2" customFormat="1">
+    <row r="185" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>17</v>
       </c>
@@ -13476,7 +13497,7 @@
       <c r="AI185"/>
       <c r="AJ185"/>
     </row>
-    <row r="186" spans="1:36" s="2" customFormat="1">
+    <row r="186" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>18</v>
       </c>
@@ -13556,7 +13577,7 @@
       <c r="AI186"/>
       <c r="AJ186"/>
     </row>
-    <row r="187" spans="1:36" s="2" customFormat="1">
+    <row r="187" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>19</v>
       </c>
@@ -13636,7 +13657,7 @@
       <c r="AI187"/>
       <c r="AJ187"/>
     </row>
-    <row r="188" spans="1:36" s="2" customFormat="1">
+    <row r="188" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>20</v>
       </c>
@@ -13716,7 +13737,7 @@
       <c r="AI188"/>
       <c r="AJ188"/>
     </row>
-    <row r="189" spans="1:36" s="2" customFormat="1">
+    <row r="189" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>21</v>
       </c>
@@ -13796,7 +13817,7 @@
       <c r="AI189"/>
       <c r="AJ189"/>
     </row>
-    <row r="190" spans="1:36" s="2" customFormat="1">
+    <row r="190" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>22</v>
       </c>
@@ -13876,7 +13897,7 @@
       <c r="AI190"/>
       <c r="AJ190"/>
     </row>
-    <row r="191" spans="1:36" s="2" customFormat="1">
+    <row r="191" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>23</v>
       </c>
@@ -13958,7 +13979,7 @@
       <c r="AI191"/>
       <c r="AJ191"/>
     </row>
-    <row r="192" spans="1:36" s="2" customFormat="1">
+    <row r="192" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>24</v>
       </c>
@@ -14038,7 +14059,7 @@
       <c r="AI192"/>
       <c r="AJ192"/>
     </row>
-    <row r="193" spans="1:36" s="2" customFormat="1">
+    <row r="193" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>25</v>
       </c>
@@ -14118,7 +14139,7 @@
       <c r="AI193"/>
       <c r="AJ193"/>
     </row>
-    <row r="194" spans="1:36" s="2" customFormat="1">
+    <row r="194" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>26</v>
       </c>
@@ -14202,7 +14223,7 @@
       <c r="AI194"/>
       <c r="AJ194"/>
     </row>
-    <row r="195" spans="1:36" s="2" customFormat="1">
+    <row r="195" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>27</v>
       </c>
@@ -14282,7 +14303,7 @@
       <c r="AI195"/>
       <c r="AJ195"/>
     </row>
-    <row r="196" spans="1:36" s="2" customFormat="1">
+    <row r="196" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>28</v>
       </c>
@@ -14362,7 +14383,7 @@
       <c r="AI196"/>
       <c r="AJ196"/>
     </row>
-    <row r="197" spans="1:36" s="2" customFormat="1">
+    <row r="197" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>29</v>
       </c>
@@ -14442,7 +14463,7 @@
       <c r="AI197"/>
       <c r="AJ197"/>
     </row>
-    <row r="198" spans="1:36" s="2" customFormat="1">
+    <row r="198" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>30</v>
       </c>
@@ -14522,7 +14543,7 @@
       <c r="AI198" s="14"/>
       <c r="AJ198"/>
     </row>
-    <row r="199" spans="1:36" s="2" customFormat="1">
+    <row r="199" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>31</v>
       </c>
@@ -14602,7 +14623,7 @@
       <c r="AI199"/>
       <c r="AJ199"/>
     </row>
-    <row r="200" spans="1:36" s="2" customFormat="1">
+    <row r="200" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>32</v>
       </c>
@@ -14682,7 +14703,7 @@
       <c r="AI200"/>
       <c r="AJ200"/>
     </row>
-    <row r="201" spans="1:36" s="2" customFormat="1">
+    <row r="201" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>33</v>
       </c>
@@ -14762,7 +14783,7 @@
       <c r="AI201"/>
       <c r="AJ201"/>
     </row>
-    <row r="202" spans="1:36" s="2" customFormat="1">
+    <row r="202" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>34</v>
       </c>
@@ -14842,7 +14863,7 @@
       <c r="AI202"/>
       <c r="AJ202"/>
     </row>
-    <row r="203" spans="1:36" s="2" customFormat="1">
+    <row r="203" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>35</v>
       </c>
@@ -14922,7 +14943,7 @@
       <c r="AI203"/>
       <c r="AJ203"/>
     </row>
-    <row r="204" spans="1:36" s="2" customFormat="1">
+    <row r="204" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>36</v>
       </c>
@@ -15002,7 +15023,7 @@
       <c r="AI204"/>
       <c r="AJ204"/>
     </row>
-    <row r="205" spans="1:36" s="2" customFormat="1">
+    <row r="205" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>58</v>
       </c>
@@ -15092,7 +15113,7 @@
       <c r="AI205"/>
       <c r="AJ205"/>
     </row>
-    <row r="206" spans="1:36" s="2" customFormat="1">
+    <row r="206" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>58</v>
       </c>
@@ -15182,7 +15203,7 @@
       <c r="AI206"/>
       <c r="AJ206"/>
     </row>
-    <row r="207" spans="1:36" s="2" customFormat="1">
+    <row r="207" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>58</v>
       </c>
@@ -15246,7 +15267,7 @@
       <c r="AI207"/>
       <c r="AJ207"/>
     </row>
-    <row r="208" spans="1:36" s="2" customFormat="1">
+    <row r="208" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>58</v>
       </c>
@@ -15336,7 +15357,7 @@
       <c r="AI208"/>
       <c r="AJ208"/>
     </row>
-    <row r="209" spans="1:36" s="2" customFormat="1">
+    <row r="209" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>58</v>
       </c>
@@ -15400,7 +15421,7 @@
       <c r="AI209"/>
       <c r="AJ209"/>
     </row>
-    <row r="210" spans="1:36" s="2" customFormat="1">
+    <row r="210" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A210"/>
       <c r="B210" t="s">
         <v>24</v>
@@ -15496,7 +15517,7 @@
       <c r="AI210"/>
       <c r="AJ210"/>
     </row>
-    <row r="211" spans="1:36" s="2" customFormat="1">
+    <row r="211" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>97</v>
       </c>
@@ -15556,7 +15577,7 @@
       <c r="AI211"/>
       <c r="AJ211"/>
     </row>
-    <row r="212" spans="1:36" s="2" customFormat="1">
+    <row r="212" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>98</v>
       </c>
@@ -15616,7 +15637,7 @@
       <c r="AI212"/>
       <c r="AJ212"/>
     </row>
-    <row r="213" spans="1:36" s="2" customFormat="1">
+    <row r="213" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>99</v>
       </c>
@@ -15676,7 +15697,7 @@
       <c r="AI213"/>
       <c r="AJ213"/>
     </row>
-    <row r="214" spans="1:36" s="2" customFormat="1">
+    <row r="214" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>100</v>
       </c>
@@ -15736,7 +15757,7 @@
       <c r="AI214"/>
       <c r="AJ214"/>
     </row>
-    <row r="215" spans="1:36" s="2" customFormat="1">
+    <row r="215" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>101</v>
       </c>
@@ -15796,7 +15817,7 @@
       <c r="AI215"/>
       <c r="AJ215"/>
     </row>
-    <row r="216" spans="1:36" s="2" customFormat="1">
+    <row r="216" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>102</v>
       </c>
@@ -15856,7 +15877,7 @@
       <c r="AI216"/>
       <c r="AJ216"/>
     </row>
-    <row r="217" spans="1:36" s="2" customFormat="1">
+    <row r="217" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>103</v>
       </c>
@@ -15916,7 +15937,7 @@
       <c r="AI217"/>
       <c r="AJ217"/>
     </row>
-    <row r="218" spans="1:36" s="2" customFormat="1">
+    <row r="218" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>104</v>
       </c>
@@ -15976,7 +15997,7 @@
       <c r="AI218"/>
       <c r="AJ218"/>
     </row>
-    <row r="219" spans="1:36" s="2" customFormat="1">
+    <row r="219" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>105</v>
       </c>
@@ -16036,7 +16057,7 @@
       <c r="AI219"/>
       <c r="AJ219"/>
     </row>
-    <row r="220" spans="1:36" s="2" customFormat="1">
+    <row r="220" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>106</v>
       </c>
@@ -16096,7 +16117,7 @@
       <c r="AI220"/>
       <c r="AJ220"/>
     </row>
-    <row r="221" spans="1:36" s="2" customFormat="1">
+    <row r="221" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>107</v>
       </c>
@@ -16156,7 +16177,7 @@
       <c r="AI221"/>
       <c r="AJ221"/>
     </row>
-    <row r="222" spans="1:36" s="2" customFormat="1">
+    <row r="222" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>108</v>
       </c>
@@ -16216,7 +16237,7 @@
       <c r="AI222"/>
       <c r="AJ222"/>
     </row>
-    <row r="223" spans="1:36" s="2" customFormat="1">
+    <row r="223" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>109</v>
       </c>
@@ -16276,7 +16297,7 @@
       <c r="AI223"/>
       <c r="AJ223"/>
     </row>
-    <row r="224" spans="1:36" s="2" customFormat="1">
+    <row r="224" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>110</v>
       </c>
@@ -16336,7 +16357,7 @@
       <c r="AI224"/>
       <c r="AJ224"/>
     </row>
-    <row r="225" spans="1:36" s="2" customFormat="1">
+    <row r="225" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>111</v>
       </c>
@@ -16396,7 +16417,7 @@
       <c r="AI225"/>
       <c r="AJ225"/>
     </row>
-    <row r="226" spans="1:36" s="2" customFormat="1">
+    <row r="226" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>112</v>
       </c>
@@ -16456,7 +16477,7 @@
       <c r="AI226"/>
       <c r="AJ226"/>
     </row>
-    <row r="227" spans="1:36" s="2" customFormat="1">
+    <row r="227" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>113</v>
       </c>
@@ -16516,7 +16537,7 @@
       <c r="AI227"/>
       <c r="AJ227"/>
     </row>
-    <row r="228" spans="1:36" s="2" customFormat="1">
+    <row r="228" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>114</v>
       </c>
@@ -16576,7 +16597,7 @@
       <c r="AI228"/>
       <c r="AJ228"/>
     </row>
-    <row r="229" spans="1:36" s="2" customFormat="1">
+    <row r="229" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>115</v>
       </c>
@@ -16636,7 +16657,7 @@
       <c r="AI229"/>
       <c r="AJ229"/>
     </row>
-    <row r="230" spans="1:36" s="2" customFormat="1">
+    <row r="230" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>116</v>
       </c>
@@ -16696,7 +16717,7 @@
       <c r="AI230"/>
       <c r="AJ230"/>
     </row>
-    <row r="231" spans="1:36" s="2" customFormat="1">
+    <row r="231" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>117</v>
       </c>
@@ -16756,7 +16777,7 @@
       <c r="AI231"/>
       <c r="AJ231"/>
     </row>
-    <row r="232" spans="1:36" s="2" customFormat="1">
+    <row r="232" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>118</v>
       </c>
@@ -16816,7 +16837,7 @@
       <c r="AI232"/>
       <c r="AJ232"/>
     </row>
-    <row r="233" spans="1:36" s="2" customFormat="1">
+    <row r="233" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>119</v>
       </c>
@@ -16876,7 +16897,7 @@
       <c r="AI233"/>
       <c r="AJ233"/>
     </row>
-    <row r="234" spans="1:36" s="17" customFormat="1">
+    <row r="234" spans="1:36" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>120</v>
       </c>
@@ -16936,7 +16957,7 @@
       <c r="AI234"/>
       <c r="AJ234"/>
     </row>
-    <row r="235" spans="1:36">
+    <row r="235" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>2</v>
       </c>
@@ -17029,7 +17050,7 @@
         <v>11.49</v>
       </c>
     </row>
-    <row r="236" spans="1:36">
+    <row r="236" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>121</v>
       </c>
@@ -17064,7 +17085,7 @@
         <v>7.69</v>
       </c>
     </row>
-    <row r="237" spans="1:36">
+    <row r="237" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>122</v>
       </c>
@@ -17099,7 +17120,7 @@
         <v>8.76</v>
       </c>
     </row>
-    <row r="238" spans="1:36">
+    <row r="238" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>123</v>
       </c>
@@ -17134,7 +17155,7 @@
         <v>10.69</v>
       </c>
     </row>
-    <row r="239" spans="1:36">
+    <row r="239" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>124</v>
       </c>
@@ -17169,7 +17190,7 @@
         <v>8.9700000000000006</v>
       </c>
     </row>
-    <row r="240" spans="1:36">
+    <row r="240" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>125</v>
       </c>
@@ -17204,7 +17225,7 @@
         <v>5.35</v>
       </c>
     </row>
-    <row r="241" spans="1:13">
+    <row r="241" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>126</v>
       </c>
@@ -17239,7 +17260,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="242" spans="1:13">
+    <row r="242" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>127</v>
       </c>
@@ -17274,7 +17295,7 @@
         <v>7.97</v>
       </c>
     </row>
-    <row r="243" spans="1:13">
+    <row r="243" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>128</v>
       </c>
@@ -17309,7 +17330,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="244" spans="1:13">
+    <row r="244" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>129</v>
       </c>
@@ -17344,7 +17365,7 @@
         <v>7.05</v>
       </c>
     </row>
-    <row r="245" spans="1:13">
+    <row r="245" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>130</v>
       </c>
@@ -17379,7 +17400,7 @@
         <v>9.5299999999999994</v>
       </c>
     </row>
-    <row r="246" spans="1:13">
+    <row r="246" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>131</v>
       </c>
@@ -17414,7 +17435,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="247" spans="1:13">
+    <row r="247" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>132</v>
       </c>
@@ -17449,7 +17470,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="248" spans="1:13">
+    <row r="248" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A248">
         <v>133</v>
       </c>
@@ -17484,7 +17505,7 @@
         <v>9.09</v>
       </c>
     </row>
-    <row r="249" spans="1:13">
+    <row r="249" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A249">
         <v>134</v>
       </c>
@@ -17519,7 +17540,7 @@
         <v>7.22</v>
       </c>
     </row>
-    <row r="250" spans="1:13">
+    <row r="250" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>135</v>
       </c>
@@ -17554,7 +17575,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="251" spans="1:13">
+    <row r="251" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A251">
         <v>136</v>
       </c>
@@ -17589,7 +17610,7 @@
         <v>8.66</v>
       </c>
     </row>
-    <row r="252" spans="1:13">
+    <row r="252" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A252">
         <v>137</v>
       </c>
@@ -17624,7 +17645,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="253" spans="1:13">
+    <row r="253" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>138</v>
       </c>
@@ -17659,7 +17680,7 @@
         <v>8.15</v>
       </c>
     </row>
-    <row r="254" spans="1:13">
+    <row r="254" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>139</v>
       </c>
@@ -17694,7 +17715,7 @@
         <v>7.65</v>
       </c>
     </row>
-    <row r="255" spans="1:13">
+    <row r="255" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A255">
         <v>140</v>
       </c>
@@ -17729,7 +17750,7 @@
         <v>13.71</v>
       </c>
     </row>
-    <row r="256" spans="1:13">
+    <row r="256" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A256">
         <v>141</v>
       </c>
@@ -17770,7 +17791,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="257" spans="1:11">
+    <row r="257" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A257">
         <v>142</v>
       </c>
@@ -17805,7 +17826,7 @@
         <v>13.07</v>
       </c>
     </row>
-    <row r="258" spans="1:11">
+    <row r="258" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A258">
         <v>143</v>
       </c>
@@ -17840,7 +17861,7 @@
         <v>13.62</v>
       </c>
     </row>
-    <row r="259" spans="1:11">
+    <row r="259" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A259">
         <v>144</v>
       </c>
@@ -17875,7 +17896,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="260" spans="1:11">
+    <row r="260" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A260">
         <v>145</v>
       </c>
@@ -17910,7 +17931,7 @@
         <v>12.43</v>
       </c>
     </row>
-    <row r="261" spans="1:11">
+    <row r="261" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A261">
         <v>146</v>
       </c>
@@ -17945,7 +17966,7 @@
         <v>11.93</v>
       </c>
     </row>
-    <row r="262" spans="1:11">
+    <row r="262" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A262">
         <v>147</v>
       </c>
@@ -17980,7 +18001,7 @@
         <v>11.56</v>
       </c>
     </row>
-    <row r="263" spans="1:11">
+    <row r="263" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A263">
         <v>148</v>
       </c>
@@ -18015,7 +18036,7 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="264" spans="1:11">
+    <row r="264" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A264">
         <v>149</v>
       </c>
@@ -18050,7 +18071,7 @@
         <v>12.22</v>
       </c>
     </row>
-    <row r="265" spans="1:11">
+    <row r="265" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A265">
         <v>150</v>
       </c>
@@ -18085,7 +18106,7 @@
         <v>12.76</v>
       </c>
     </row>
-    <row r="266" spans="1:11">
+    <row r="266" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A266">
         <v>151</v>
       </c>
@@ -18120,7 +18141,7 @@
         <v>12.62</v>
       </c>
     </row>
-    <row r="267" spans="1:11">
+    <row r="267" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A267">
         <v>152</v>
       </c>
@@ -18155,7 +18176,7 @@
         <v>13.84</v>
       </c>
     </row>
-    <row r="268" spans="1:11">
+    <row r="268" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A268">
         <v>153</v>
       </c>
@@ -18190,7 +18211,7 @@
         <v>12.63</v>
       </c>
     </row>
-    <row r="269" spans="1:11">
+    <row r="269" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A269">
         <v>154</v>
       </c>
@@ -18225,7 +18246,7 @@
         <v>12.04</v>
       </c>
     </row>
-    <row r="270" spans="1:11">
+    <row r="270" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A270">
         <v>155</v>
       </c>
@@ -18260,7 +18281,7 @@
         <v>12.41</v>
       </c>
     </row>
-    <row r="271" spans="1:11">
+    <row r="271" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A271">
         <v>156</v>
       </c>
@@ -18295,7 +18316,7 @@
         <v>18.010000000000002</v>
       </c>
     </row>
-    <row r="272" spans="1:11">
+    <row r="272" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A272">
         <v>157</v>
       </c>
@@ -18330,7 +18351,7 @@
         <v>20.57</v>
       </c>
     </row>
-    <row r="273" spans="1:36">
+    <row r="273" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A273" s="2">
         <v>158</v>
       </c>
@@ -18392,7 +18413,7 @@
       <c r="AI273" s="2"/>
       <c r="AJ273" s="2"/>
     </row>
-    <row r="274" spans="1:36">
+    <row r="274" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A274" s="17"/>
       <c r="B274" s="17"/>
       <c r="C274" s="17"/>
@@ -18430,7 +18451,7 @@
       <c r="AI274" s="17"/>
       <c r="AJ274" s="17"/>
     </row>
-    <row r="275" spans="1:36">
+    <row r="275" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>58</v>
       </c>
@@ -18510,7 +18531,7 @@
         <v>17.149999999999999</v>
       </c>
     </row>
-    <row r="276" spans="1:36">
+    <row r="276" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>58</v>
       </c>
@@ -18590,7 +18611,7 @@
         <v>15.75</v>
       </c>
     </row>
-    <row r="277" spans="1:36">
+    <row r="277" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>58</v>
       </c>
@@ -18670,7 +18691,7 @@
         <v>20.45</v>
       </c>
     </row>
-    <row r="278" spans="1:36">
+    <row r="278" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>58</v>
       </c>
@@ -18751,7 +18772,7 @@
       </c>
       <c r="AA278" s="2"/>
     </row>
-    <row r="279" spans="1:36">
+    <row r="279" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>58</v>
       </c>
@@ -18831,7 +18852,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="280" spans="1:36">
+    <row r="280" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>58</v>
       </c>
@@ -18861,7 +18882,7 @@
       </c>
       <c r="J280" s="2"/>
     </row>
-    <row r="281" spans="1:36">
+    <row r="281" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>58</v>
       </c>
@@ -18941,7 +18962,7 @@
         <v>16.579999999999998</v>
       </c>
     </row>
-    <row r="282" spans="1:36">
+    <row r="282" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>58</v>
       </c>
@@ -19021,7 +19042,7 @@
         <v>11.88</v>
       </c>
     </row>
-    <row r="283" spans="1:36">
+    <row r="283" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>58</v>
       </c>
@@ -19101,7 +19122,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="284" spans="1:36">
+    <row r="284" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>58</v>
       </c>
@@ -19181,7 +19202,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="285" spans="1:36">
+    <row r="285" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>58</v>
       </c>
@@ -19261,7 +19282,7 @@
         <v>8.0500000000000007</v>
       </c>
     </row>
-    <row r="286" spans="1:36">
+    <row r="286" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>58</v>
       </c>
@@ -19341,7 +19362,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="287" spans="1:36">
+    <row r="287" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>58</v>
       </c>
@@ -19421,7 +19442,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="288" spans="1:36">
+    <row r="288" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>58</v>
       </c>
@@ -19501,7 +19522,7 @@
         <v>4.3499999999999996</v>
       </c>
     </row>
-    <row r="289" spans="1:26">
+    <row r="289" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>58</v>
       </c>
@@ -19581,7 +19602,7 @@
         <v>5.92</v>
       </c>
     </row>
-    <row r="290" spans="1:26">
+    <row r="290" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>58</v>
       </c>
@@ -19661,7 +19682,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="291" spans="1:26">
+    <row r="291" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>58</v>
       </c>
@@ -19741,7 +19762,7 @@
         <v>5.75</v>
       </c>
     </row>
-    <row r="292" spans="1:26">
+    <row r="292" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>58</v>
       </c>
@@ -19821,7 +19842,7 @@
         <v>4.45</v>
       </c>
     </row>
-    <row r="293" spans="1:26">
+    <row r="293" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>58</v>
       </c>
@@ -19871,7 +19892,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="294" spans="1:26">
+    <row r="294" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>58</v>
       </c>
@@ -19951,7 +19972,7 @@
         <v>5.95</v>
       </c>
     </row>
-    <row r="295" spans="1:26">
+    <row r="295" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>58</v>
       </c>
@@ -20031,7 +20052,7 @@
         <v>6.95</v>
       </c>
     </row>
-    <row r="296" spans="1:26">
+    <row r="296" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>58</v>
       </c>
@@ -20111,7 +20132,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="297" spans="1:26">
+    <row r="297" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>58</v>
       </c>
@@ -20191,7 +20212,7 @@
         <v>10.52</v>
       </c>
     </row>
-    <row r="298" spans="1:26">
+    <row r="298" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>58</v>
       </c>
@@ -20271,7 +20292,7 @@
         <v>6.85</v>
       </c>
     </row>
-    <row r="299" spans="1:26">
+    <row r="299" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>58</v>
       </c>
@@ -20351,7 +20372,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="300" spans="1:26">
+    <row r="300" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>58</v>
       </c>
@@ -20431,7 +20452,7 @@
         <v>4.45</v>
       </c>
     </row>
-    <row r="301" spans="1:26">
+    <row r="301" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>58</v>
       </c>
@@ -20511,7 +20532,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="302" spans="1:26">
+    <row r="302" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>58</v>
       </c>
@@ -20591,7 +20612,7 @@
         <v>3.62</v>
       </c>
     </row>
-    <row r="303" spans="1:26">
+    <row r="303" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>58</v>
       </c>
@@ -20671,7 +20692,7 @@
         <v>10.65</v>
       </c>
     </row>
-    <row r="304" spans="1:26">
+    <row r="304" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>58</v>
       </c>
@@ -20751,7 +20772,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="305" spans="1:30">
+    <row r="305" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>58</v>
       </c>
@@ -20831,7 +20852,7 @@
         <v>2.89</v>
       </c>
     </row>
-    <row r="306" spans="1:30">
+    <row r="306" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>58</v>
       </c>
@@ -20911,7 +20932,7 @@
         <v>5.82</v>
       </c>
     </row>
-    <row r="307" spans="1:30">
+    <row r="307" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>58</v>
       </c>
@@ -20991,7 +21012,7 @@
         <v>6.25</v>
       </c>
     </row>
-    <row r="308" spans="1:30">
+    <row r="308" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>58</v>
       </c>
@@ -21071,7 +21092,7 @@
         <v>12.42</v>
       </c>
     </row>
-    <row r="309" spans="1:30">
+    <row r="309" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>58</v>
       </c>
@@ -21151,7 +21172,7 @@
         <v>12.17</v>
       </c>
     </row>
-    <row r="310" spans="1:30">
+    <row r="310" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>58</v>
       </c>
@@ -21183,7 +21204,7 @@
         <v>8.7799999999999994</v>
       </c>
     </row>
-    <row r="311" spans="1:30">
+    <row r="311" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>58</v>
       </c>
@@ -21275,7 +21296,7 @@
         <v>13.09</v>
       </c>
     </row>
-    <row r="312" spans="1:30">
+    <row r="312" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>58</v>
       </c>
@@ -21352,7 +21373,7 @@
         <v>12.94</v>
       </c>
     </row>
-    <row r="313" spans="1:30">
+    <row r="313" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>58</v>
       </c>
@@ -21384,7 +21405,7 @@
         <v>18.79</v>
       </c>
     </row>
-    <row r="314" spans="1:30">
+    <row r="314" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>58</v>
       </c>
@@ -21476,7 +21497,7 @@
         <v>13.19</v>
       </c>
     </row>
-    <row r="315" spans="1:30">
+    <row r="315" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>58</v>
       </c>
@@ -21556,7 +21577,7 @@
         <v>13.68</v>
       </c>
     </row>
-    <row r="316" spans="1:30">
+    <row r="316" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>58</v>
       </c>
@@ -21636,7 +21657,7 @@
         <v>8.99</v>
       </c>
     </row>
-    <row r="317" spans="1:30">
+    <row r="317" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>58</v>
       </c>
@@ -21716,7 +21737,7 @@
         <v>8.98</v>
       </c>
     </row>
-    <row r="318" spans="1:30">
+    <row r="318" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>58</v>
       </c>
@@ -21796,7 +21817,7 @@
         <v>10.48</v>
       </c>
     </row>
-    <row r="319" spans="1:30">
+    <row r="319" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>58</v>
       </c>
@@ -21876,7 +21897,7 @@
         <v>9.1300000000000008</v>
       </c>
     </row>
-    <row r="320" spans="1:30">
+    <row r="320" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>58</v>
       </c>
@@ -21956,7 +21977,7 @@
         <v>7.39</v>
       </c>
     </row>
-    <row r="321" spans="1:26">
+    <row r="321" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>58</v>
       </c>
@@ -22036,7 +22057,7 @@
         <v>9.64</v>
       </c>
     </row>
-    <row r="322" spans="1:26">
+    <row r="322" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>58</v>
       </c>
@@ -22116,7 +22137,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="323" spans="1:26">
+    <row r="323" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>58</v>
       </c>
@@ -22164,6 +22185,712 @@
       </c>
       <c r="P323">
         <v>5.9</v>
+      </c>
+    </row>
+    <row r="324" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A324" t="s">
+        <v>58</v>
+      </c>
+      <c r="B324" t="s">
+        <v>12</v>
+      </c>
+      <c r="C324" t="s">
+        <v>59</v>
+      </c>
+      <c r="D324" t="s">
+        <v>61</v>
+      </c>
+      <c r="E324" t="s">
+        <v>58</v>
+      </c>
+      <c r="F324" t="s">
+        <v>58</v>
+      </c>
+      <c r="G324">
+        <v>2</v>
+      </c>
+      <c r="H324">
+        <v>2</v>
+      </c>
+      <c r="I324">
+        <v>2</v>
+      </c>
+      <c r="J324">
+        <v>2</v>
+      </c>
+      <c r="K324">
+        <v>2</v>
+      </c>
+      <c r="L324">
+        <v>2</v>
+      </c>
+      <c r="M324">
+        <v>2</v>
+      </c>
+      <c r="N324">
+        <v>2</v>
+      </c>
+      <c r="O324">
+        <v>2</v>
+      </c>
+      <c r="P324">
+        <v>2</v>
+      </c>
+      <c r="Q324">
+        <v>2</v>
+      </c>
+      <c r="R324">
+        <v>2</v>
+      </c>
+      <c r="S324">
+        <v>2</v>
+      </c>
+      <c r="T324">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="325" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A325" t="s">
+        <v>58</v>
+      </c>
+      <c r="B325" t="s">
+        <v>13</v>
+      </c>
+      <c r="C325" t="s">
+        <v>59</v>
+      </c>
+      <c r="D325" t="s">
+        <v>65</v>
+      </c>
+      <c r="E325" t="s">
+        <v>58</v>
+      </c>
+      <c r="F325" t="s">
+        <v>58</v>
+      </c>
+      <c r="G325">
+        <v>2</v>
+      </c>
+      <c r="H325">
+        <v>2</v>
+      </c>
+      <c r="I325">
+        <v>2</v>
+      </c>
+      <c r="J325">
+        <v>2</v>
+      </c>
+      <c r="K325">
+        <v>2</v>
+      </c>
+      <c r="L325">
+        <v>2</v>
+      </c>
+      <c r="M325">
+        <v>2</v>
+      </c>
+      <c r="N325">
+        <v>2</v>
+      </c>
+      <c r="O325">
+        <v>2</v>
+      </c>
+      <c r="P325">
+        <v>2</v>
+      </c>
+      <c r="Q325">
+        <v>2</v>
+      </c>
+      <c r="R325">
+        <v>2</v>
+      </c>
+      <c r="S325">
+        <v>2</v>
+      </c>
+      <c r="T325">
+        <v>2</v>
+      </c>
+      <c r="U325">
+        <v>2</v>
+      </c>
+      <c r="V325">
+        <v>2</v>
+      </c>
+      <c r="W325">
+        <v>2</v>
+      </c>
+      <c r="X325">
+        <v>2</v>
+      </c>
+      <c r="Y325">
+        <v>2</v>
+      </c>
+      <c r="Z325">
+        <v>2</v>
+      </c>
+      <c r="AA325">
+        <v>2</v>
+      </c>
+      <c r="AB325">
+        <v>2</v>
+      </c>
+      <c r="AC325">
+        <v>2</v>
+      </c>
+      <c r="AD325">
+        <v>2</v>
+      </c>
+      <c r="AE325">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="326" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A326" t="s">
+        <v>58</v>
+      </c>
+      <c r="B326" t="s">
+        <v>13</v>
+      </c>
+      <c r="C326" t="s">
+        <v>59</v>
+      </c>
+      <c r="D326" t="s">
+        <v>65</v>
+      </c>
+      <c r="E326" t="s">
+        <v>58</v>
+      </c>
+      <c r="F326" t="s">
+        <v>58</v>
+      </c>
+      <c r="G326">
+        <v>2</v>
+      </c>
+      <c r="H326">
+        <v>2</v>
+      </c>
+      <c r="I326">
+        <v>2</v>
+      </c>
+      <c r="J326">
+        <v>2</v>
+      </c>
+      <c r="K326">
+        <v>2</v>
+      </c>
+      <c r="L326">
+        <v>2</v>
+      </c>
+      <c r="M326">
+        <v>2</v>
+      </c>
+      <c r="N326">
+        <v>2</v>
+      </c>
+      <c r="O326">
+        <v>2</v>
+      </c>
+      <c r="P326">
+        <v>2</v>
+      </c>
+      <c r="Q326">
+        <v>2</v>
+      </c>
+      <c r="R326">
+        <v>2</v>
+      </c>
+      <c r="S326">
+        <v>2</v>
+      </c>
+      <c r="T326">
+        <v>2</v>
+      </c>
+      <c r="U326">
+        <v>2</v>
+      </c>
+      <c r="V326">
+        <v>2</v>
+      </c>
+      <c r="W326">
+        <v>2</v>
+      </c>
+      <c r="X326">
+        <v>2</v>
+      </c>
+      <c r="Y326">
+        <v>2</v>
+      </c>
+      <c r="Z326">
+        <v>2</v>
+      </c>
+      <c r="AA326">
+        <v>2</v>
+      </c>
+      <c r="AB326">
+        <v>2</v>
+      </c>
+      <c r="AC326">
+        <v>2</v>
+      </c>
+      <c r="AD326">
+        <v>2</v>
+      </c>
+      <c r="AE326">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="327" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A327" t="s">
+        <v>58</v>
+      </c>
+      <c r="B327" t="s">
+        <v>13</v>
+      </c>
+      <c r="C327" t="s">
+        <v>59</v>
+      </c>
+      <c r="D327" t="s">
+        <v>65</v>
+      </c>
+      <c r="E327" t="s">
+        <v>58</v>
+      </c>
+      <c r="F327" t="s">
+        <v>58</v>
+      </c>
+      <c r="G327">
+        <v>2</v>
+      </c>
+      <c r="H327">
+        <v>2</v>
+      </c>
+      <c r="I327">
+        <v>2</v>
+      </c>
+      <c r="J327">
+        <v>2</v>
+      </c>
+      <c r="K327">
+        <v>2</v>
+      </c>
+      <c r="L327">
+        <v>2</v>
+      </c>
+      <c r="M327">
+        <v>2</v>
+      </c>
+      <c r="N327">
+        <v>2</v>
+      </c>
+      <c r="O327">
+        <v>2</v>
+      </c>
+      <c r="P327">
+        <v>2</v>
+      </c>
+      <c r="Q327">
+        <v>2</v>
+      </c>
+      <c r="R327">
+        <v>2</v>
+      </c>
+      <c r="S327">
+        <v>2</v>
+      </c>
+      <c r="T327">
+        <v>2</v>
+      </c>
+      <c r="U327">
+        <v>2</v>
+      </c>
+      <c r="V327">
+        <v>2</v>
+      </c>
+      <c r="W327">
+        <v>2</v>
+      </c>
+      <c r="X327">
+        <v>2</v>
+      </c>
+      <c r="Y327">
+        <v>2</v>
+      </c>
+      <c r="Z327">
+        <v>2</v>
+      </c>
+      <c r="AA327">
+        <v>2</v>
+      </c>
+      <c r="AB327">
+        <v>2</v>
+      </c>
+      <c r="AC327">
+        <v>2</v>
+      </c>
+      <c r="AD327">
+        <v>2</v>
+      </c>
+      <c r="AE327">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="328" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A328" t="s">
+        <v>58</v>
+      </c>
+      <c r="B328" t="s">
+        <v>13</v>
+      </c>
+      <c r="C328" t="s">
+        <v>59</v>
+      </c>
+      <c r="D328" t="s">
+        <v>65</v>
+      </c>
+      <c r="E328" t="s">
+        <v>58</v>
+      </c>
+      <c r="F328" t="s">
+        <v>58</v>
+      </c>
+      <c r="G328">
+        <v>2</v>
+      </c>
+      <c r="H328">
+        <v>2</v>
+      </c>
+      <c r="I328">
+        <v>2</v>
+      </c>
+      <c r="J328">
+        <v>2</v>
+      </c>
+      <c r="K328">
+        <v>2</v>
+      </c>
+      <c r="L328">
+        <v>2</v>
+      </c>
+      <c r="M328">
+        <v>2</v>
+      </c>
+      <c r="N328">
+        <v>2</v>
+      </c>
+      <c r="O328">
+        <v>2</v>
+      </c>
+      <c r="P328">
+        <v>2</v>
+      </c>
+      <c r="Q328">
+        <v>2</v>
+      </c>
+      <c r="R328">
+        <v>2</v>
+      </c>
+      <c r="S328">
+        <v>2</v>
+      </c>
+      <c r="T328">
+        <v>2</v>
+      </c>
+      <c r="U328">
+        <v>2</v>
+      </c>
+      <c r="V328">
+        <v>2</v>
+      </c>
+      <c r="W328">
+        <v>2</v>
+      </c>
+      <c r="X328">
+        <v>2</v>
+      </c>
+      <c r="Y328">
+        <v>2</v>
+      </c>
+      <c r="Z328">
+        <v>2</v>
+      </c>
+      <c r="AA328">
+        <v>2</v>
+      </c>
+      <c r="AB328">
+        <v>2</v>
+      </c>
+      <c r="AC328">
+        <v>2</v>
+      </c>
+      <c r="AD328">
+        <v>2</v>
+      </c>
+      <c r="AE328">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="329" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A329" t="s">
+        <v>58</v>
+      </c>
+      <c r="B329" t="s">
+        <v>13</v>
+      </c>
+      <c r="C329" t="s">
+        <v>59</v>
+      </c>
+      <c r="D329" t="s">
+        <v>65</v>
+      </c>
+      <c r="E329" t="s">
+        <v>58</v>
+      </c>
+      <c r="F329" t="s">
+        <v>58</v>
+      </c>
+      <c r="G329">
+        <v>2</v>
+      </c>
+      <c r="H329">
+        <v>2</v>
+      </c>
+      <c r="I329">
+        <v>2</v>
+      </c>
+      <c r="J329">
+        <v>2</v>
+      </c>
+      <c r="K329">
+        <v>2</v>
+      </c>
+      <c r="L329">
+        <v>2</v>
+      </c>
+      <c r="M329">
+        <v>2</v>
+      </c>
+      <c r="N329">
+        <v>2</v>
+      </c>
+      <c r="O329">
+        <v>2</v>
+      </c>
+      <c r="P329">
+        <v>2</v>
+      </c>
+      <c r="Q329">
+        <v>2</v>
+      </c>
+      <c r="R329">
+        <v>2</v>
+      </c>
+      <c r="S329">
+        <v>2</v>
+      </c>
+      <c r="T329">
+        <v>2</v>
+      </c>
+      <c r="U329">
+        <v>2</v>
+      </c>
+      <c r="V329">
+        <v>2</v>
+      </c>
+      <c r="W329">
+        <v>2</v>
+      </c>
+      <c r="X329">
+        <v>2</v>
+      </c>
+      <c r="Y329">
+        <v>2</v>
+      </c>
+      <c r="Z329">
+        <v>2</v>
+      </c>
+      <c r="AA329">
+        <v>2</v>
+      </c>
+      <c r="AB329">
+        <v>2</v>
+      </c>
+      <c r="AC329">
+        <v>2</v>
+      </c>
+      <c r="AD329">
+        <v>2</v>
+      </c>
+      <c r="AE329">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="330" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A330" t="s">
+        <v>58</v>
+      </c>
+      <c r="B330" t="s">
+        <v>13</v>
+      </c>
+      <c r="C330" t="s">
+        <v>59</v>
+      </c>
+      <c r="D330" t="s">
+        <v>65</v>
+      </c>
+      <c r="E330" t="s">
+        <v>58</v>
+      </c>
+      <c r="F330" t="s">
+        <v>58</v>
+      </c>
+      <c r="G330">
+        <v>2</v>
+      </c>
+      <c r="H330">
+        <v>2</v>
+      </c>
+      <c r="I330">
+        <v>2</v>
+      </c>
+      <c r="J330">
+        <v>2</v>
+      </c>
+      <c r="K330">
+        <v>2</v>
+      </c>
+      <c r="L330">
+        <v>2</v>
+      </c>
+      <c r="M330">
+        <v>2</v>
+      </c>
+      <c r="N330">
+        <v>2</v>
+      </c>
+      <c r="O330">
+        <v>2</v>
+      </c>
+      <c r="P330">
+        <v>2</v>
+      </c>
+      <c r="Q330">
+        <v>2</v>
+      </c>
+      <c r="R330">
+        <v>2</v>
+      </c>
+      <c r="S330">
+        <v>2</v>
+      </c>
+      <c r="T330">
+        <v>2</v>
+      </c>
+      <c r="U330">
+        <v>2</v>
+      </c>
+      <c r="V330">
+        <v>2</v>
+      </c>
+      <c r="W330">
+        <v>2</v>
+      </c>
+      <c r="X330">
+        <v>2</v>
+      </c>
+      <c r="Y330">
+        <v>2</v>
+      </c>
+      <c r="Z330">
+        <v>2</v>
+      </c>
+      <c r="AA330">
+        <v>2</v>
+      </c>
+      <c r="AB330">
+        <v>2</v>
+      </c>
+      <c r="AC330">
+        <v>2</v>
+      </c>
+      <c r="AD330">
+        <v>2</v>
+      </c>
+      <c r="AE330">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="331" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A331" t="s">
+        <v>58</v>
+      </c>
+      <c r="B331" t="s">
+        <v>13</v>
+      </c>
+      <c r="C331" t="s">
+        <v>59</v>
+      </c>
+      <c r="D331" t="s">
+        <v>65</v>
+      </c>
+      <c r="E331" t="s">
+        <v>58</v>
+      </c>
+      <c r="F331" t="s">
+        <v>58</v>
+      </c>
+      <c r="G331">
+        <v>2</v>
+      </c>
+      <c r="H331">
+        <v>2</v>
+      </c>
+      <c r="I331">
+        <v>2</v>
+      </c>
+      <c r="J331">
+        <v>2</v>
+      </c>
+      <c r="K331">
+        <v>2</v>
+      </c>
+      <c r="L331">
+        <v>2</v>
+      </c>
+      <c r="M331">
+        <v>2</v>
+      </c>
+      <c r="N331">
+        <v>2</v>
+      </c>
+      <c r="O331">
+        <v>2</v>
+      </c>
+      <c r="P331">
+        <v>2</v>
+      </c>
+      <c r="Q331">
+        <v>2</v>
+      </c>
+      <c r="R331">
+        <v>2</v>
+      </c>
+      <c r="S331">
+        <v>2</v>
+      </c>
+      <c r="T331">
+        <v>2</v>
+      </c>
+      <c r="U331">
+        <v>2</v>
+      </c>
+      <c r="V331">
+        <v>2</v>
+      </c>
+      <c r="W331">
+        <v>2</v>
+      </c>
+      <c r="X331">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>